<commit_message>
update figures for report
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo(1).xlsx
+++ b/Data_inputs/LAFPP_PlanInfo(1).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_LAFPP\Data_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="9" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="Death_dec" sheetId="5" r:id="rId19"/>
     <sheet name="DROP cashflow" sheetId="25" r:id="rId20"/>
     <sheet name="GASB_cashflow" sheetId="26" r:id="rId21"/>
-    <sheet name="Sheet1" sheetId="28" r:id="rId22"/>
+    <sheet name="Fiscal" sheetId="28" r:id="rId22"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="274">
   <si>
     <t>Notes</t>
   </si>
@@ -2279,16 +2279,38 @@
   <si>
     <t>Only model this type.</t>
   </si>
+  <si>
+    <t>GenFund.original</t>
+  </si>
+  <si>
+    <t>Growth.high</t>
+  </si>
+  <si>
+    <t>Grwoth.med</t>
+  </si>
+  <si>
+    <t>Growth.low</t>
+  </si>
+  <si>
+    <t>GenFund.high</t>
+  </si>
+  <si>
+    <t>GenFund.med</t>
+  </si>
+  <si>
+    <t>GenFund.low</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -2526,7 +2548,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2947,6 +2969,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3587,6 +3613,95 @@
         <a:xfrm>
           <a:off x="609600" y="5448300"/>
           <a:ext cx="5123809" cy="3047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>153035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD917F8D-B860-40A3-8350-AF9CE6B6D8C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8134350" y="1009650"/>
+          <a:ext cx="6400800" cy="6382385"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C5E8274-BA4A-4C79-9D15-7B4D79744420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8439150" y="7562850"/>
+          <a:ext cx="6229350" cy="6648450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14069,7 +14184,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14648,13 +14763,597 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" t="s">
+        <v>273</v>
+      </c>
+      <c r="I5" t="s">
+        <v>268</v>
+      </c>
+      <c r="J5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2015</v>
+      </c>
+      <c r="D6" s="160">
+        <f>D7/(1+0.044)</f>
+        <v>5324062.2605363978</v>
+      </c>
+      <c r="E6" s="160">
+        <f t="shared" ref="E6:G6" si="0">E7/(1+0.044)</f>
+        <v>5324062.2605363978</v>
+      </c>
+      <c r="F6" s="160">
+        <f t="shared" si="0"/>
+        <v>5324062.2605363978</v>
+      </c>
+      <c r="G6" s="160">
+        <f t="shared" si="0"/>
+        <v>5324062.2605363978</v>
+      </c>
+      <c r="I6" t="s">
+        <v>269</v>
+      </c>
+      <c r="J6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2016</v>
+      </c>
+      <c r="D7" s="161">
+        <v>5558321</v>
+      </c>
+      <c r="E7" s="161">
+        <v>5558321</v>
+      </c>
+      <c r="F7" s="161">
+        <v>5558321</v>
+      </c>
+      <c r="G7" s="161">
+        <v>5558321</v>
+      </c>
+      <c r="I7" t="s">
+        <v>270</v>
+      </c>
+      <c r="J7" s="162">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2017</v>
+      </c>
+      <c r="D8" s="161">
+        <v>5600426</v>
+      </c>
+      <c r="E8" s="161">
+        <v>5600426</v>
+      </c>
+      <c r="F8" s="161">
+        <v>5600426</v>
+      </c>
+      <c r="G8" s="161">
+        <v>5600426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="161">
+        <v>5783199</v>
+      </c>
+      <c r="E9" s="161">
+        <v>5783199</v>
+      </c>
+      <c r="F9" s="161">
+        <v>5783199</v>
+      </c>
+      <c r="G9" s="161">
+        <v>5783199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2019</v>
+      </c>
+      <c r="D10" s="161">
+        <v>5983030</v>
+      </c>
+      <c r="E10" s="161">
+        <v>5983030</v>
+      </c>
+      <c r="F10" s="161">
+        <v>5983030</v>
+      </c>
+      <c r="G10" s="161">
+        <v>5983030</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2020</v>
+      </c>
+      <c r="D11" s="161">
+        <v>6156556</v>
+      </c>
+      <c r="E11" s="161">
+        <v>6156556</v>
+      </c>
+      <c r="F11" s="161">
+        <v>6156556</v>
+      </c>
+      <c r="G11" s="161">
+        <v>6156556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2021</v>
+      </c>
+      <c r="D12" s="161"/>
+      <c r="E12" s="163">
+        <f>E11*(1 + $J$5)</f>
+        <v>6372035.46</v>
+      </c>
+      <c r="F12" s="163">
+        <f>F11*(1 + $J$6)</f>
+        <v>6335096.1239999998</v>
+      </c>
+      <c r="G12" s="163">
+        <f>G11*(1 + $J$7)</f>
+        <v>6279687.1200000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="E13" s="163">
+        <f t="shared" ref="E13:E35" si="1">E12*(1 + J$5)</f>
+        <v>6595056.7010999992</v>
+      </c>
+      <c r="F13" s="163">
+        <f t="shared" ref="F13:F35" si="2">F12*(1 + $J$6)</f>
+        <v>6518813.9115959993</v>
+      </c>
+      <c r="G13" s="163">
+        <f t="shared" ref="G13:G35" si="3">G12*(1 + $J$7)</f>
+        <v>6405280.8624</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2023</v>
+      </c>
+      <c r="E14" s="163">
+        <f t="shared" si="1"/>
+        <v>6825883.6856384985</v>
+      </c>
+      <c r="F14" s="163">
+        <f t="shared" si="2"/>
+        <v>6707859.515032283</v>
+      </c>
+      <c r="G14" s="163">
+        <f t="shared" si="3"/>
+        <v>6533386.4796480006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>2024</v>
+      </c>
+      <c r="E15" s="163">
+        <f t="shared" si="1"/>
+        <v>7064789.6146358456</v>
+      </c>
+      <c r="F15" s="163">
+        <f t="shared" si="2"/>
+        <v>6902387.4409682183</v>
+      </c>
+      <c r="G15" s="163">
+        <f t="shared" si="3"/>
+        <v>6664054.2092409609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2025</v>
+      </c>
+      <c r="E16" s="163">
+        <f t="shared" si="1"/>
+        <v>7312057.2511481</v>
+      </c>
+      <c r="F16" s="163">
+        <f t="shared" si="2"/>
+        <v>7102556.6767562963</v>
+      </c>
+      <c r="G16" s="163">
+        <f t="shared" si="3"/>
+        <v>6797335.2934257798</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2026</v>
+      </c>
+      <c r="E17" s="163">
+        <f t="shared" si="1"/>
+        <v>7567979.254938283</v>
+      </c>
+      <c r="F17" s="163">
+        <f t="shared" si="2"/>
+        <v>7308530.8203822281</v>
+      </c>
+      <c r="G17" s="163">
+        <f t="shared" si="3"/>
+        <v>6933281.9992942959</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2027</v>
+      </c>
+      <c r="E18" s="163">
+        <f t="shared" si="1"/>
+        <v>7832858.5288611222</v>
+      </c>
+      <c r="F18" s="163">
+        <f t="shared" si="2"/>
+        <v>7520478.2141733123</v>
+      </c>
+      <c r="G18" s="163">
+        <f t="shared" si="3"/>
+        <v>7071947.6392801823</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2028</v>
+      </c>
+      <c r="E19" s="163">
+        <f t="shared" si="1"/>
+        <v>8107008.5773712611</v>
+      </c>
+      <c r="F19" s="163">
+        <f t="shared" si="2"/>
+        <v>7738572.0823843377</v>
+      </c>
+      <c r="G19" s="163">
+        <f t="shared" si="3"/>
+        <v>7213386.592065786</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2029</v>
+      </c>
+      <c r="E20" s="163">
+        <f t="shared" si="1"/>
+        <v>8390753.877579255</v>
+      </c>
+      <c r="F20" s="163">
+        <f t="shared" si="2"/>
+        <v>7962990.6727734832</v>
+      </c>
+      <c r="G20" s="163">
+        <f t="shared" si="3"/>
+        <v>7357654.3239071015</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2030</v>
+      </c>
+      <c r="E21" s="163">
+        <f t="shared" si="1"/>
+        <v>8684430.2632945292</v>
+      </c>
+      <c r="F21" s="163">
+        <f t="shared" si="2"/>
+        <v>8193917.4022839135</v>
+      </c>
+      <c r="G21" s="163">
+        <f t="shared" si="3"/>
+        <v>7504807.4103852436</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2031</v>
+      </c>
+      <c r="E22" s="163">
+        <f t="shared" si="1"/>
+        <v>8988385.3225098364</v>
+      </c>
+      <c r="F22" s="163">
+        <f t="shared" si="2"/>
+        <v>8431541.0069501456</v>
+      </c>
+      <c r="G22" s="163">
+        <f t="shared" si="3"/>
+        <v>7654903.5585929491</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2032</v>
+      </c>
+      <c r="E23" s="163">
+        <f t="shared" si="1"/>
+        <v>9302978.8087976798</v>
+      </c>
+      <c r="F23" s="163">
+        <f t="shared" si="2"/>
+        <v>8676055.6961516999</v>
+      </c>
+      <c r="G23" s="163">
+        <f t="shared" si="3"/>
+        <v>7808001.6297648083</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2033</v>
+      </c>
+      <c r="E24" s="163">
+        <f t="shared" si="1"/>
+        <v>9628583.0671055987</v>
+      </c>
+      <c r="F24" s="163">
+        <f t="shared" si="2"/>
+        <v>8927661.3113400992</v>
+      </c>
+      <c r="G24" s="163">
+        <f t="shared" si="3"/>
+        <v>7964161.6623601047</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2034</v>
+      </c>
+      <c r="E25" s="163">
+        <f t="shared" si="1"/>
+        <v>9965583.474454293</v>
+      </c>
+      <c r="F25" s="163">
+        <f t="shared" si="2"/>
+        <v>9186563.4893689621</v>
+      </c>
+      <c r="G25" s="163">
+        <f t="shared" si="3"/>
+        <v>8123444.8956073066</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2035</v>
+      </c>
+      <c r="E26" s="163">
+        <f t="shared" si="1"/>
+        <v>10314378.896060193</v>
+      </c>
+      <c r="F26" s="163">
+        <f t="shared" si="2"/>
+        <v>9452973.8305606619</v>
+      </c>
+      <c r="G26" s="163">
+        <f t="shared" si="3"/>
+        <v>8285913.7935194531</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2036</v>
+      </c>
+      <c r="E27" s="163">
+        <f t="shared" si="1"/>
+        <v>10675382.157422299</v>
+      </c>
+      <c r="F27" s="163">
+        <f t="shared" si="2"/>
+        <v>9727110.0716469195</v>
+      </c>
+      <c r="G27" s="163">
+        <f t="shared" si="3"/>
+        <v>8451632.0693898425</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2037</v>
+      </c>
+      <c r="E28" s="163">
+        <f t="shared" si="1"/>
+        <v>11049020.532932078</v>
+      </c>
+      <c r="F28" s="163">
+        <f t="shared" si="2"/>
+        <v>10009196.263724679</v>
+      </c>
+      <c r="G28" s="163">
+        <f t="shared" si="3"/>
+        <v>8620664.7107776403</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>2038</v>
+      </c>
+      <c r="E29" s="163">
+        <f t="shared" si="1"/>
+        <v>11435736.251584701</v>
+      </c>
+      <c r="F29" s="163">
+        <f t="shared" si="2"/>
+        <v>10299462.955372695</v>
+      </c>
+      <c r="G29" s="163">
+        <f t="shared" si="3"/>
+        <v>8793078.0049931929</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>2039</v>
+      </c>
+      <c r="E30" s="163">
+        <f t="shared" si="1"/>
+        <v>11835987.020390164</v>
+      </c>
+      <c r="F30" s="163">
+        <f t="shared" si="2"/>
+        <v>10598147.381078502</v>
+      </c>
+      <c r="G30" s="163">
+        <f t="shared" si="3"/>
+        <v>8968939.5650930572</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>2040</v>
+      </c>
+      <c r="E31" s="163">
+        <f t="shared" si="1"/>
+        <v>12250246.56610382</v>
+      </c>
+      <c r="F31" s="163">
+        <f t="shared" si="2"/>
+        <v>10905493.655129777</v>
+      </c>
+      <c r="G31" s="163">
+        <f t="shared" si="3"/>
+        <v>9148318.3563949186</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>2041</v>
+      </c>
+      <c r="E32" s="163">
+        <f t="shared" si="1"/>
+        <v>12679005.195917452</v>
+      </c>
+      <c r="F32" s="163">
+        <f t="shared" si="2"/>
+        <v>11221752.97112854</v>
+      </c>
+      <c r="G32" s="163">
+        <f t="shared" si="3"/>
+        <v>9331284.7235228177</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>2042</v>
+      </c>
+      <c r="E33" s="163">
+        <f t="shared" si="1"/>
+        <v>13122770.377774561</v>
+      </c>
+      <c r="F33" s="163">
+        <f t="shared" si="2"/>
+        <v>11547183.807291267</v>
+      </c>
+      <c r="G33" s="163">
+        <f t="shared" si="3"/>
+        <v>9517910.4179932736</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2043</v>
+      </c>
+      <c r="E34" s="163">
+        <f t="shared" si="1"/>
+        <v>13582067.34099667</v>
+      </c>
+      <c r="F34" s="163">
+        <f t="shared" si="2"/>
+        <v>11882052.137702713</v>
+      </c>
+      <c r="G34" s="163">
+        <f t="shared" si="3"/>
+        <v>9708268.6263531391</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>2044</v>
+      </c>
+      <c r="E35" s="163">
+        <f t="shared" si="1"/>
+        <v>14057439.697931552</v>
+      </c>
+      <c r="F35" s="163">
+        <f t="shared" si="2"/>
+        <v>12226631.649696091</v>
+      </c>
+      <c r="G35" s="163">
+        <f t="shared" si="3"/>
+        <v>9902433.998880202</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14697,7 +15396,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add fiscal analysis for LAFPP
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_PlanInfo(1).xlsx
+++ b/Data_inputs/LAFPP_PlanInfo(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="9" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="711" firstSheet="10" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="22" r:id="rId1"/>
@@ -34,6 +34,8 @@
     <sheet name="DROP cashflow" sheetId="25" r:id="rId20"/>
     <sheet name="GASB_cashflow" sheetId="26" r:id="rId21"/>
     <sheet name="Fiscal" sheetId="28" r:id="rId22"/>
+    <sheet name="Fiscal2" sheetId="29" r:id="rId23"/>
+    <sheet name="Fiscal3" sheetId="30" r:id="rId24"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -44,8 +46,150 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yimeng Yin</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yimeng Yin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+AV2015 pdf p60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yimeng Yin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1 year lag of the expected EEC in the AV
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yimeng Yin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+AV2016 pdf p75</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yimeng Yin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+6220076
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yimeng Yin</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yimeng Yin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+AV2015 pdf p60</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="290">
   <si>
     <t>Notes</t>
   </si>
@@ -2300,6 +2444,57 @@
   <si>
     <t>GenFund.low</t>
   </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>D35</t>
+  </si>
+  <si>
+    <t>ERC including Health subsidy</t>
+  </si>
+  <si>
+    <t>FY ending in</t>
+  </si>
+  <si>
+    <t>model year</t>
+  </si>
+  <si>
+    <t>actual EEC + ERC of pension</t>
+  </si>
+  <si>
+    <t>expected EEC</t>
+  </si>
+  <si>
+    <t>estimated actual ERC</t>
+  </si>
+  <si>
+    <t>Est. pensin ERC / total ERC</t>
+  </si>
+  <si>
+    <t>ERC including Health subsidy
+(AV)</t>
+  </si>
+  <si>
+    <t>ERC including health subsidy
+(budget)</t>
+  </si>
+  <si>
+    <t>LAFPP</t>
+  </si>
+  <si>
+    <t>LACERS</t>
+  </si>
+  <si>
+    <t>growth rate</t>
+  </si>
+  <si>
+    <t>ADC(?) of pension</t>
+  </si>
+  <si>
+    <t>ERC:
+LACERS/LAFPP</t>
+  </si>
 </sst>
 </file>
 
@@ -2310,9 +2505,9 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2477,8 +2672,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2500,6 +2708,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2548,7 +2762,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2924,6 +3138,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2969,10 +3212,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3708,6 +3953,170 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91DB36F5-0252-44FB-B5B2-0B24476D638E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1009650" y="3228975"/>
+          <a:ext cx="6705600" cy="1466850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Assume pension ERC accounts for 75% of the total ERC (pension + health).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E82900EC-116D-4794-9940-434685ED4D6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1428750" y="3286125"/>
+          <a:ext cx="8496300" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>We</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> assume the total contribution of LACERS is about 85% of </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t>LAPFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5038,15 +5447,15 @@
       <c r="A5" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="145" t="s">
+      <c r="C5" s="161"/>
+      <c r="D5" s="158" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
       <c r="G5" s="42" t="s">
         <v>78</v>
       </c>
@@ -5069,10 +5478,10 @@
       <c r="E6" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="149" t="s">
+      <c r="F6" s="162" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="149"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="42"/>
       <c r="I6" s="42"/>
     </row>
@@ -5096,10 +5505,10 @@
       <c r="C9" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="146" t="s">
+      <c r="D9" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="146"/>
+      <c r="E9" s="159"/>
       <c r="F9" s="38" t="s">
         <v>64</v>
       </c>
@@ -5111,16 +5520,16 @@
       <c r="A10" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="163" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="150"/>
-      <c r="D10" s="150" t="s">
+      <c r="C10" s="163"/>
+      <c r="D10" s="163" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="150"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="150"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -5131,18 +5540,18 @@
       <c r="A12" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="159" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="146" t="s">
+      <c r="C12" s="161"/>
+      <c r="D12" s="159" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146" t="s">
+      <c r="E12" s="159"/>
+      <c r="F12" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="146"/>
+      <c r="G12" s="159"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
@@ -5312,22 +5721,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="151" t="s">
+      <c r="A5" s="164" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="165" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152" t="s">
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="165"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="151"/>
+      <c r="A6" s="164"/>
       <c r="B6" s="57" t="s">
         <v>93</v>
       </c>
@@ -8049,10 +8458,10 @@
       <c r="E4" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="F4" s="146" t="s">
+      <c r="F4" s="159" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="148"/>
+      <c r="G4" s="161"/>
     </row>
     <row r="5" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
@@ -8070,21 +8479,21 @@
       <c r="E5" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="146" t="s">
+      <c r="F5" s="159" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="146"/>
+      <c r="G5" s="159"/>
     </row>
     <row r="6" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="153" t="s">
+      <c r="A6" s="166" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="153"/>
-      <c r="C6" s="153"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="166"/>
+      <c r="E6" s="166"/>
+      <c r="F6" s="166"/>
+      <c r="G6" s="166"/>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -8696,30 +9105,30 @@
       <c r="A4" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
     </row>
     <row r="5" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="160" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="147"/>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="304.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155" t="s">
+      <c r="A7" s="168" t="s">
         <v>202</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -8728,10 +9137,10 @@
       <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="146" t="s">
+      <c r="D7" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="148"/>
+      <c r="E7" s="161"/>
       <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
@@ -8740,15 +9149,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="156" t="s">
+      <c r="A8" s="168"/>
+      <c r="B8" s="169" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="157"/>
-      <c r="D8" s="157"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="157"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
+      <c r="G8" s="170"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -9048,10 +9457,10 @@
       <c r="D5" s="98" t="s">
         <v>264</v>
       </c>
-      <c r="E5" s="158" t="s">
+      <c r="E5" s="171" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="158"/>
+      <c r="F5" s="171"/>
       <c r="G5" s="98" t="s">
         <v>199</v>
       </c>
@@ -9069,10 +9478,10 @@
       <c r="D6" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="158" t="s">
+      <c r="E6" s="171" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="158"/>
+      <c r="F6" s="171"/>
       <c r="G6" s="98" t="s">
         <v>197</v>
       </c>
@@ -9093,10 +9502,10 @@
       <c r="D7" s="98" t="s">
         <v>194</v>
       </c>
-      <c r="E7" s="158" t="s">
+      <c r="E7" s="171" t="s">
         <v>198</v>
       </c>
-      <c r="F7" s="158"/>
+      <c r="F7" s="171"/>
       <c r="G7" s="98" t="s">
         <v>198</v>
       </c>
@@ -9493,7 +9902,7 @@
   <dimension ref="B2:W109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="T114" sqref="T114"/>
@@ -9531,24 +9940,24 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="J5" s="159" t="s">
+      <c r="J5" s="172" t="s">
         <v>170</v>
       </c>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
-      <c r="M5" s="159"/>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159" t="s">
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
+      <c r="O5" s="172"/>
+      <c r="P5" s="172"/>
+      <c r="Q5" s="172" t="s">
         <v>183</v>
       </c>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="159"/>
-      <c r="U5" s="159"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="R5" s="172"/>
+      <c r="S5" s="172"/>
+      <c r="T5" s="172"/>
+      <c r="U5" s="172"/>
+      <c r="V5" s="172"/>
+      <c r="W5" s="172"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -14765,8 +15174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14789,7 +15198,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -14797,10 +15206,13 @@
         <v>87</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
       <c r="D5" s="6" t="s">
         <v>267</v>
       </c>
@@ -14824,19 +15236,19 @@
       <c r="C6">
         <v>2015</v>
       </c>
-      <c r="D6" s="160">
+      <c r="D6" s="146">
         <f>D7/(1+0.044)</f>
         <v>5324062.2605363978</v>
       </c>
-      <c r="E6" s="160">
+      <c r="E6" s="146">
         <f t="shared" ref="E6:G6" si="0">E7/(1+0.044)</f>
         <v>5324062.2605363978</v>
       </c>
-      <c r="F6" s="160">
+      <c r="F6" s="146">
         <f t="shared" si="0"/>
         <v>5324062.2605363978</v>
       </c>
-      <c r="G6" s="160">
+      <c r="G6" s="146">
         <f t="shared" si="0"/>
         <v>5324062.2605363978</v>
       </c>
@@ -14851,22 +15263,22 @@
       <c r="C7">
         <v>2016</v>
       </c>
-      <c r="D7" s="161">
+      <c r="D7" s="147">
         <v>5558321</v>
       </c>
-      <c r="E7" s="161">
+      <c r="E7" s="147">
         <v>5558321</v>
       </c>
-      <c r="F7" s="161">
+      <c r="F7" s="147">
         <v>5558321</v>
       </c>
-      <c r="G7" s="161">
+      <c r="G7" s="147">
         <v>5558321</v>
       </c>
       <c r="I7" t="s">
         <v>270</v>
       </c>
-      <c r="J7" s="162">
+      <c r="J7" s="148">
         <v>0.02</v>
       </c>
     </row>
@@ -14874,16 +15286,16 @@
       <c r="C8">
         <v>2017</v>
       </c>
-      <c r="D8" s="161">
+      <c r="D8" s="147">
         <v>5600426</v>
       </c>
-      <c r="E8" s="161">
+      <c r="E8" s="147">
         <v>5600426</v>
       </c>
-      <c r="F8" s="161">
+      <c r="F8" s="147">
         <v>5600426</v>
       </c>
-      <c r="G8" s="161">
+      <c r="G8" s="147">
         <v>5600426</v>
       </c>
     </row>
@@ -14891,16 +15303,16 @@
       <c r="C9">
         <v>2018</v>
       </c>
-      <c r="D9" s="161">
+      <c r="D9" s="147">
         <v>5783199</v>
       </c>
-      <c r="E9" s="161">
+      <c r="E9" s="147">
         <v>5783199</v>
       </c>
-      <c r="F9" s="161">
+      <c r="F9" s="147">
         <v>5783199</v>
       </c>
-      <c r="G9" s="161">
+      <c r="G9" s="147">
         <v>5783199</v>
       </c>
     </row>
@@ -14908,16 +15320,16 @@
       <c r="C10">
         <v>2019</v>
       </c>
-      <c r="D10" s="161">
+      <c r="D10" s="147">
         <v>5983030</v>
       </c>
-      <c r="E10" s="161">
+      <c r="E10" s="147">
         <v>5983030</v>
       </c>
-      <c r="F10" s="161">
+      <c r="F10" s="147">
         <v>5983030</v>
       </c>
-      <c r="G10" s="161">
+      <c r="G10" s="147">
         <v>5983030</v>
       </c>
     </row>
@@ -14925,16 +15337,16 @@
       <c r="C11">
         <v>2020</v>
       </c>
-      <c r="D11" s="161">
+      <c r="D11" s="147">
         <v>6156556</v>
       </c>
-      <c r="E11" s="161">
+      <c r="E11" s="147">
         <v>6156556</v>
       </c>
-      <c r="F11" s="161">
+      <c r="F11" s="147">
         <v>6156556</v>
       </c>
-      <c r="G11" s="161">
+      <c r="G11" s="147">
         <v>6156556</v>
       </c>
     </row>
@@ -14942,16 +15354,16 @@
       <c r="C12">
         <v>2021</v>
       </c>
-      <c r="D12" s="161"/>
-      <c r="E12" s="163">
+      <c r="D12" s="147"/>
+      <c r="E12" s="149">
         <f>E11*(1 + $J$5)</f>
         <v>6372035.46</v>
       </c>
-      <c r="F12" s="163">
+      <c r="F12" s="149">
         <f>F11*(1 + $J$6)</f>
         <v>6335096.1239999998</v>
       </c>
-      <c r="G12" s="163">
+      <c r="G12" s="149">
         <f>G11*(1 + $J$7)</f>
         <v>6279687.1200000001</v>
       </c>
@@ -14960,15 +15372,15 @@
       <c r="C13">
         <v>2022</v>
       </c>
-      <c r="E13" s="163">
+      <c r="E13" s="149">
         <f t="shared" ref="E13:E35" si="1">E12*(1 + J$5)</f>
         <v>6595056.7010999992</v>
       </c>
-      <c r="F13" s="163">
+      <c r="F13" s="149">
         <f t="shared" ref="F13:F35" si="2">F12*(1 + $J$6)</f>
         <v>6518813.9115959993</v>
       </c>
-      <c r="G13" s="163">
+      <c r="G13" s="149">
         <f t="shared" ref="G13:G35" si="3">G12*(1 + $J$7)</f>
         <v>6405280.8624</v>
       </c>
@@ -14977,15 +15389,15 @@
       <c r="C14">
         <v>2023</v>
       </c>
-      <c r="E14" s="163">
+      <c r="E14" s="149">
         <f t="shared" si="1"/>
         <v>6825883.6856384985</v>
       </c>
-      <c r="F14" s="163">
+      <c r="F14" s="149">
         <f t="shared" si="2"/>
         <v>6707859.515032283</v>
       </c>
-      <c r="G14" s="163">
+      <c r="G14" s="149">
         <f t="shared" si="3"/>
         <v>6533386.4796480006</v>
       </c>
@@ -14994,15 +15406,15 @@
       <c r="C15">
         <v>2024</v>
       </c>
-      <c r="E15" s="163">
+      <c r="E15" s="149">
         <f t="shared" si="1"/>
         <v>7064789.6146358456</v>
       </c>
-      <c r="F15" s="163">
+      <c r="F15" s="149">
         <f t="shared" si="2"/>
         <v>6902387.4409682183</v>
       </c>
-      <c r="G15" s="163">
+      <c r="G15" s="149">
         <f t="shared" si="3"/>
         <v>6664054.2092409609</v>
       </c>
@@ -15011,15 +15423,15 @@
       <c r="C16">
         <v>2025</v>
       </c>
-      <c r="E16" s="163">
+      <c r="E16" s="149">
         <f t="shared" si="1"/>
         <v>7312057.2511481</v>
       </c>
-      <c r="F16" s="163">
+      <c r="F16" s="149">
         <f t="shared" si="2"/>
         <v>7102556.6767562963</v>
       </c>
-      <c r="G16" s="163">
+      <c r="G16" s="149">
         <f t="shared" si="3"/>
         <v>6797335.2934257798</v>
       </c>
@@ -15028,15 +15440,15 @@
       <c r="C17">
         <v>2026</v>
       </c>
-      <c r="E17" s="163">
+      <c r="E17" s="149">
         <f t="shared" si="1"/>
         <v>7567979.254938283</v>
       </c>
-      <c r="F17" s="163">
+      <c r="F17" s="149">
         <f t="shared" si="2"/>
         <v>7308530.8203822281</v>
       </c>
-      <c r="G17" s="163">
+      <c r="G17" s="149">
         <f t="shared" si="3"/>
         <v>6933281.9992942959</v>
       </c>
@@ -15045,15 +15457,15 @@
       <c r="C18">
         <v>2027</v>
       </c>
-      <c r="E18" s="163">
+      <c r="E18" s="149">
         <f t="shared" si="1"/>
         <v>7832858.5288611222</v>
       </c>
-      <c r="F18" s="163">
+      <c r="F18" s="149">
         <f t="shared" si="2"/>
         <v>7520478.2141733123</v>
       </c>
-      <c r="G18" s="163">
+      <c r="G18" s="149">
         <f t="shared" si="3"/>
         <v>7071947.6392801823</v>
       </c>
@@ -15062,15 +15474,15 @@
       <c r="C19">
         <v>2028</v>
       </c>
-      <c r="E19" s="163">
+      <c r="E19" s="149">
         <f t="shared" si="1"/>
         <v>8107008.5773712611</v>
       </c>
-      <c r="F19" s="163">
+      <c r="F19" s="149">
         <f t="shared" si="2"/>
         <v>7738572.0823843377</v>
       </c>
-      <c r="G19" s="163">
+      <c r="G19" s="149">
         <f t="shared" si="3"/>
         <v>7213386.592065786</v>
       </c>
@@ -15079,15 +15491,15 @@
       <c r="C20">
         <v>2029</v>
       </c>
-      <c r="E20" s="163">
+      <c r="E20" s="149">
         <f t="shared" si="1"/>
         <v>8390753.877579255</v>
       </c>
-      <c r="F20" s="163">
+      <c r="F20" s="149">
         <f t="shared" si="2"/>
         <v>7962990.6727734832</v>
       </c>
-      <c r="G20" s="163">
+      <c r="G20" s="149">
         <f t="shared" si="3"/>
         <v>7357654.3239071015</v>
       </c>
@@ -15096,15 +15508,15 @@
       <c r="C21">
         <v>2030</v>
       </c>
-      <c r="E21" s="163">
+      <c r="E21" s="149">
         <f t="shared" si="1"/>
         <v>8684430.2632945292</v>
       </c>
-      <c r="F21" s="163">
+      <c r="F21" s="149">
         <f t="shared" si="2"/>
         <v>8193917.4022839135</v>
       </c>
-      <c r="G21" s="163">
+      <c r="G21" s="149">
         <f t="shared" si="3"/>
         <v>7504807.4103852436</v>
       </c>
@@ -15113,15 +15525,15 @@
       <c r="C22">
         <v>2031</v>
       </c>
-      <c r="E22" s="163">
+      <c r="E22" s="149">
         <f t="shared" si="1"/>
         <v>8988385.3225098364</v>
       </c>
-      <c r="F22" s="163">
+      <c r="F22" s="149">
         <f t="shared" si="2"/>
         <v>8431541.0069501456</v>
       </c>
-      <c r="G22" s="163">
+      <c r="G22" s="149">
         <f t="shared" si="3"/>
         <v>7654903.5585929491</v>
       </c>
@@ -15130,15 +15542,15 @@
       <c r="C23">
         <v>2032</v>
       </c>
-      <c r="E23" s="163">
+      <c r="E23" s="149">
         <f t="shared" si="1"/>
         <v>9302978.8087976798</v>
       </c>
-      <c r="F23" s="163">
+      <c r="F23" s="149">
         <f t="shared" si="2"/>
         <v>8676055.6961516999</v>
       </c>
-      <c r="G23" s="163">
+      <c r="G23" s="149">
         <f t="shared" si="3"/>
         <v>7808001.6297648083</v>
       </c>
@@ -15147,15 +15559,15 @@
       <c r="C24">
         <v>2033</v>
       </c>
-      <c r="E24" s="163">
+      <c r="E24" s="149">
         <f t="shared" si="1"/>
         <v>9628583.0671055987</v>
       </c>
-      <c r="F24" s="163">
+      <c r="F24" s="149">
         <f t="shared" si="2"/>
         <v>8927661.3113400992</v>
       </c>
-      <c r="G24" s="163">
+      <c r="G24" s="149">
         <f t="shared" si="3"/>
         <v>7964161.6623601047</v>
       </c>
@@ -15164,15 +15576,15 @@
       <c r="C25">
         <v>2034</v>
       </c>
-      <c r="E25" s="163">
+      <c r="E25" s="149">
         <f t="shared" si="1"/>
         <v>9965583.474454293</v>
       </c>
-      <c r="F25" s="163">
+      <c r="F25" s="149">
         <f t="shared" si="2"/>
         <v>9186563.4893689621</v>
       </c>
-      <c r="G25" s="163">
+      <c r="G25" s="149">
         <f t="shared" si="3"/>
         <v>8123444.8956073066</v>
       </c>
@@ -15181,15 +15593,15 @@
       <c r="C26">
         <v>2035</v>
       </c>
-      <c r="E26" s="163">
+      <c r="E26" s="149">
         <f t="shared" si="1"/>
         <v>10314378.896060193</v>
       </c>
-      <c r="F26" s="163">
+      <c r="F26" s="149">
         <f t="shared" si="2"/>
         <v>9452973.8305606619</v>
       </c>
-      <c r="G26" s="163">
+      <c r="G26" s="149">
         <f t="shared" si="3"/>
         <v>8285913.7935194531</v>
       </c>
@@ -15198,15 +15610,15 @@
       <c r="C27">
         <v>2036</v>
       </c>
-      <c r="E27" s="163">
+      <c r="E27" s="149">
         <f t="shared" si="1"/>
         <v>10675382.157422299</v>
       </c>
-      <c r="F27" s="163">
+      <c r="F27" s="149">
         <f t="shared" si="2"/>
         <v>9727110.0716469195</v>
       </c>
-      <c r="G27" s="163">
+      <c r="G27" s="149">
         <f t="shared" si="3"/>
         <v>8451632.0693898425</v>
       </c>
@@ -15215,15 +15627,15 @@
       <c r="C28">
         <v>2037</v>
       </c>
-      <c r="E28" s="163">
+      <c r="E28" s="149">
         <f t="shared" si="1"/>
         <v>11049020.532932078</v>
       </c>
-      <c r="F28" s="163">
+      <c r="F28" s="149">
         <f t="shared" si="2"/>
         <v>10009196.263724679</v>
       </c>
-      <c r="G28" s="163">
+      <c r="G28" s="149">
         <f t="shared" si="3"/>
         <v>8620664.7107776403</v>
       </c>
@@ -15232,15 +15644,15 @@
       <c r="C29">
         <v>2038</v>
       </c>
-      <c r="E29" s="163">
+      <c r="E29" s="149">
         <f t="shared" si="1"/>
         <v>11435736.251584701</v>
       </c>
-      <c r="F29" s="163">
+      <c r="F29" s="149">
         <f t="shared" si="2"/>
         <v>10299462.955372695</v>
       </c>
-      <c r="G29" s="163">
+      <c r="G29" s="149">
         <f t="shared" si="3"/>
         <v>8793078.0049931929</v>
       </c>
@@ -15249,15 +15661,15 @@
       <c r="C30">
         <v>2039</v>
       </c>
-      <c r="E30" s="163">
+      <c r="E30" s="149">
         <f t="shared" si="1"/>
         <v>11835987.020390164</v>
       </c>
-      <c r="F30" s="163">
+      <c r="F30" s="149">
         <f t="shared" si="2"/>
         <v>10598147.381078502</v>
       </c>
-      <c r="G30" s="163">
+      <c r="G30" s="149">
         <f t="shared" si="3"/>
         <v>8968939.5650930572</v>
       </c>
@@ -15266,15 +15678,15 @@
       <c r="C31">
         <v>2040</v>
       </c>
-      <c r="E31" s="163">
+      <c r="E31" s="149">
         <f t="shared" si="1"/>
         <v>12250246.56610382</v>
       </c>
-      <c r="F31" s="163">
+      <c r="F31" s="149">
         <f t="shared" si="2"/>
         <v>10905493.655129777</v>
       </c>
-      <c r="G31" s="163">
+      <c r="G31" s="149">
         <f t="shared" si="3"/>
         <v>9148318.3563949186</v>
       </c>
@@ -15283,15 +15695,15 @@
       <c r="C32">
         <v>2041</v>
       </c>
-      <c r="E32" s="163">
+      <c r="E32" s="149">
         <f t="shared" si="1"/>
         <v>12679005.195917452</v>
       </c>
-      <c r="F32" s="163">
+      <c r="F32" s="149">
         <f t="shared" si="2"/>
         <v>11221752.97112854</v>
       </c>
-      <c r="G32" s="163">
+      <c r="G32" s="149">
         <f t="shared" si="3"/>
         <v>9331284.7235228177</v>
       </c>
@@ -15300,15 +15712,15 @@
       <c r="C33">
         <v>2042</v>
       </c>
-      <c r="E33" s="163">
+      <c r="E33" s="149">
         <f t="shared" si="1"/>
         <v>13122770.377774561</v>
       </c>
-      <c r="F33" s="163">
+      <c r="F33" s="149">
         <f t="shared" si="2"/>
         <v>11547183.807291267</v>
       </c>
-      <c r="G33" s="163">
+      <c r="G33" s="149">
         <f t="shared" si="3"/>
         <v>9517910.4179932736</v>
       </c>
@@ -15317,15 +15729,15 @@
       <c r="C34">
         <v>2043</v>
       </c>
-      <c r="E34" s="163">
+      <c r="E34" s="149">
         <f t="shared" si="1"/>
         <v>13582067.34099667</v>
       </c>
-      <c r="F34" s="163">
+      <c r="F34" s="149">
         <f t="shared" si="2"/>
         <v>11882052.137702713</v>
       </c>
-      <c r="G34" s="163">
+      <c r="G34" s="149">
         <f t="shared" si="3"/>
         <v>9708268.6263531391</v>
       </c>
@@ -15334,15 +15746,15 @@
       <c r="C35">
         <v>2044</v>
       </c>
-      <c r="E35" s="163">
+      <c r="E35" s="149">
         <f t="shared" si="1"/>
         <v>14057439.697931552</v>
       </c>
-      <c r="F35" s="163">
+      <c r="F35" s="149">
         <f t="shared" si="2"/>
         <v>12226631.649696091</v>
       </c>
-      <c r="G35" s="163">
+      <c r="G35" s="149">
         <f t="shared" si="3"/>
         <v>9902433.998880202</v>
       </c>
@@ -15354,6 +15766,655 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="151" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="151" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="145" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="145" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="145" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="145" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="145" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="145"/>
+      <c r="J2" s="37" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2005</v>
+      </c>
+      <c r="C3" s="154">
+        <v>2006</v>
+      </c>
+      <c r="D3" s="152"/>
+      <c r="E3" s="155">
+        <v>223219844</v>
+      </c>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="153">
+        <v>143945802</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2006</v>
+      </c>
+      <c r="C4" s="154">
+        <v>2007</v>
+      </c>
+      <c r="D4" s="155">
+        <v>286167278</v>
+      </c>
+      <c r="E4" s="155">
+        <v>314980319</v>
+      </c>
+      <c r="F4" s="155">
+        <v>91545104</v>
+      </c>
+      <c r="G4" s="155">
+        <f t="shared" ref="G4:G8" si="0">E4-F4</f>
+        <v>223435215</v>
+      </c>
+      <c r="H4" s="156">
+        <f t="shared" ref="H4:H8" si="1">G4/D4</f>
+        <v>0.78078533842712794</v>
+      </c>
+      <c r="I4" s="155"/>
+      <c r="J4" s="153">
+        <v>224946082</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2007</v>
+      </c>
+      <c r="C5" s="154">
+        <v>2008</v>
+      </c>
+      <c r="D5" s="155">
+        <v>333672743</v>
+      </c>
+      <c r="E5" s="155">
+        <v>354299709</v>
+      </c>
+      <c r="F5" s="155">
+        <v>95700124</v>
+      </c>
+      <c r="G5" s="155">
+        <f t="shared" si="0"/>
+        <v>258599585</v>
+      </c>
+      <c r="H5" s="156">
+        <f t="shared" si="1"/>
+        <v>0.77500961773194643</v>
+      </c>
+      <c r="I5" s="155"/>
+      <c r="J5" s="153">
+        <v>261635491</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2008</v>
+      </c>
+      <c r="C6" s="154">
+        <v>2009</v>
+      </c>
+      <c r="D6" s="155">
+        <v>326876839</v>
+      </c>
+      <c r="E6" s="155">
+        <v>342383376</v>
+      </c>
+      <c r="F6" s="155">
+        <v>102485719</v>
+      </c>
+      <c r="G6" s="155">
+        <f t="shared" si="0"/>
+        <v>239897657</v>
+      </c>
+      <c r="H6" s="156">
+        <f t="shared" si="1"/>
+        <v>0.73390839722357937</v>
+      </c>
+      <c r="I6" s="155"/>
+      <c r="J6" s="153">
+        <v>238697929</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2009</v>
+      </c>
+      <c r="C7" s="154">
+        <v>2010</v>
+      </c>
+      <c r="D7" s="155">
+        <v>357165140</v>
+      </c>
+      <c r="E7" s="155">
+        <v>356928488</v>
+      </c>
+      <c r="F7" s="155">
+        <v>112286300</v>
+      </c>
+      <c r="G7" s="155">
+        <f t="shared" si="0"/>
+        <v>244642188</v>
+      </c>
+      <c r="H7" s="156">
+        <f t="shared" si="1"/>
+        <v>0.68495539066326572</v>
+      </c>
+      <c r="I7" s="155"/>
+      <c r="J7" s="153">
+        <v>250516858</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="154">
+        <v>2011</v>
+      </c>
+      <c r="D8" s="155">
+        <v>388773459</v>
+      </c>
+      <c r="E8" s="155">
+        <v>382563515</v>
+      </c>
+      <c r="F8" s="155">
+        <v>111732379</v>
+      </c>
+      <c r="G8" s="155">
+        <f t="shared" si="0"/>
+        <v>270831136</v>
+      </c>
+      <c r="H8" s="156">
+        <f t="shared" si="1"/>
+        <v>0.69662969456976231</v>
+      </c>
+      <c r="I8" s="155"/>
+      <c r="J8" s="153">
+        <v>277092251</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2011</v>
+      </c>
+      <c r="C9" s="154">
+        <v>2012</v>
+      </c>
+      <c r="D9" s="155">
+        <v>444565284</v>
+      </c>
+      <c r="E9" s="155">
+        <v>441692557</v>
+      </c>
+      <c r="F9" s="155">
+        <v>110770763</v>
+      </c>
+      <c r="G9" s="155">
+        <f>E9-F9</f>
+        <v>330921794</v>
+      </c>
+      <c r="H9" s="156">
+        <f>G9/D9</f>
+        <v>0.74437165003644323</v>
+      </c>
+      <c r="I9" s="155"/>
+      <c r="J9" s="153">
+        <v>321593433</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2012</v>
+      </c>
+      <c r="C10" s="154">
+        <v>2013</v>
+      </c>
+      <c r="D10" s="155">
+        <v>508387283</v>
+      </c>
+      <c r="E10" s="155">
+        <v>497225747</v>
+      </c>
+      <c r="F10" s="155">
+        <v>127343851</v>
+      </c>
+      <c r="G10" s="155">
+        <f t="shared" ref="G10:G12" si="2">E10-F10</f>
+        <v>369881896</v>
+      </c>
+      <c r="H10" s="156">
+        <f t="shared" ref="H10:H12" si="3">G10/D10</f>
+        <v>0.72755930049493389</v>
+      </c>
+      <c r="I10" s="155"/>
+      <c r="J10" s="153">
+        <v>375448092</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2013</v>
+      </c>
+      <c r="C11" s="154">
+        <v>2014</v>
+      </c>
+      <c r="D11" s="155">
+        <v>578805107</v>
+      </c>
+      <c r="E11" s="155">
+        <v>565093149</v>
+      </c>
+      <c r="F11" s="155">
+        <v>129370345</v>
+      </c>
+      <c r="G11" s="155">
+        <f t="shared" si="2"/>
+        <v>435722804</v>
+      </c>
+      <c r="H11" s="156">
+        <f t="shared" si="3"/>
+        <v>0.75279709651905335</v>
+      </c>
+      <c r="I11" s="155"/>
+      <c r="J11" s="153">
+        <v>440698260</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2014</v>
+      </c>
+      <c r="C12" s="154">
+        <v>2015</v>
+      </c>
+      <c r="D12" s="155">
+        <v>628808763</v>
+      </c>
+      <c r="E12" s="155">
+        <v>626119974</v>
+      </c>
+      <c r="F12" s="155">
+        <v>132691115</v>
+      </c>
+      <c r="G12" s="155">
+        <f t="shared" si="2"/>
+        <v>493428859</v>
+      </c>
+      <c r="H12" s="156">
+        <f t="shared" si="3"/>
+        <v>0.78470417086092681</v>
+      </c>
+      <c r="I12" s="155"/>
+      <c r="J12" s="153">
+        <v>480332251</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2014</v>
+      </c>
+      <c r="C13" s="154">
+        <v>2015</v>
+      </c>
+      <c r="F13" s="155">
+        <v>134441085</v>
+      </c>
+      <c r="G13" s="155"/>
+      <c r="H13" s="156"/>
+      <c r="I13" s="155"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E2" s="173" t="s">
+        <v>285</v>
+      </c>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="174" t="s">
+        <v>286</v>
+      </c>
+      <c r="I2" s="174"/>
+    </row>
+    <row r="3" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C3" s="151" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="151" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="145" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="151" t="s">
+        <v>284</v>
+      </c>
+      <c r="G3" s="150" t="s">
+        <v>287</v>
+      </c>
+      <c r="H3" s="151" t="s">
+        <v>284</v>
+      </c>
+      <c r="I3" s="150" t="s">
+        <v>287</v>
+      </c>
+      <c r="J3" s="150" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2005</v>
+      </c>
+      <c r="D4" s="154">
+        <v>2006</v>
+      </c>
+      <c r="E4" s="152"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="J4" s="157"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2006</v>
+      </c>
+      <c r="D5" s="154">
+        <v>2007</v>
+      </c>
+      <c r="E5" s="155">
+        <v>286167278</v>
+      </c>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="J5" s="157"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2007</v>
+      </c>
+      <c r="D6" s="154">
+        <v>2008</v>
+      </c>
+      <c r="E6" s="155">
+        <v>333672743</v>
+      </c>
+      <c r="F6" s="155"/>
+      <c r="G6" s="155"/>
+      <c r="H6" s="155"/>
+      <c r="J6" s="157"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2008</v>
+      </c>
+      <c r="D7" s="154">
+        <v>2009</v>
+      </c>
+      <c r="E7" s="155">
+        <v>326876839</v>
+      </c>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="155"/>
+      <c r="J7" s="157"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2009</v>
+      </c>
+      <c r="D8" s="154">
+        <v>2010</v>
+      </c>
+      <c r="E8" s="155">
+        <v>357165140</v>
+      </c>
+      <c r="F8" s="155"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="155"/>
+      <c r="J8" s="157"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2010</v>
+      </c>
+      <c r="D9" s="154">
+        <v>2011</v>
+      </c>
+      <c r="E9" s="155">
+        <v>388773459</v>
+      </c>
+      <c r="F9" s="155">
+        <f>394.7*1000000</f>
+        <v>394700000</v>
+      </c>
+      <c r="G9" s="155"/>
+      <c r="H9" s="155">
+        <f>335.4*1000000</f>
+        <v>335400000</v>
+      </c>
+      <c r="J9" s="157">
+        <f>H9/F9</f>
+        <v>0.84975931086901446</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2011</v>
+      </c>
+      <c r="D10" s="154">
+        <v>2012</v>
+      </c>
+      <c r="E10" s="155">
+        <v>444565284</v>
+      </c>
+      <c r="F10" s="155">
+        <f>471384436+3644894+736292</f>
+        <v>475765622</v>
+      </c>
+      <c r="G10" s="155"/>
+      <c r="H10" s="155">
+        <v>482498572</v>
+      </c>
+      <c r="J10" s="157">
+        <f t="shared" ref="J10:J14" si="0">H10/F10</f>
+        <v>1.0141518211671039</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2012</v>
+      </c>
+      <c r="D11" s="154">
+        <v>2013</v>
+      </c>
+      <c r="E11" s="155">
+        <v>508387283</v>
+      </c>
+      <c r="F11" s="155">
+        <f>505082619+1003643+3498111</f>
+        <v>509584373</v>
+      </c>
+      <c r="G11" s="157">
+        <f>F11/F10-1</f>
+        <v>7.108279673052964E-2</v>
+      </c>
+      <c r="H11" s="155">
+        <v>419806102</v>
+      </c>
+      <c r="I11" s="157">
+        <f>H11/H10-1</f>
+        <v>-0.12993296485859862</v>
+      </c>
+      <c r="J11" s="157">
+        <f t="shared" si="0"/>
+        <v>0.82382059624108606</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2013</v>
+      </c>
+      <c r="D12" s="154">
+        <v>2014</v>
+      </c>
+      <c r="E12" s="155">
+        <v>578805107</v>
+      </c>
+      <c r="F12" s="155">
+        <f>574871226+1070154+3933881</f>
+        <v>579875261</v>
+      </c>
+      <c r="G12" s="157">
+        <f t="shared" ref="G12:G14" si="1">F12/F11-1</f>
+        <v>0.13793768357963354</v>
+      </c>
+      <c r="H12" s="155">
+        <v>450746001</v>
+      </c>
+      <c r="I12" s="157">
+        <f t="shared" ref="I12:I14" si="2">H12/H11-1</f>
+        <v>7.3700450881011736E-2</v>
+      </c>
+      <c r="J12" s="157">
+        <f t="shared" si="0"/>
+        <v>0.77731545267629554</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2014</v>
+      </c>
+      <c r="D13" s="154">
+        <v>2015</v>
+      </c>
+      <c r="E13" s="155">
+        <v>628808763</v>
+      </c>
+      <c r="F13" s="155">
+        <f>624423315+551000+4385448</f>
+        <v>629359763</v>
+      </c>
+      <c r="G13" s="157">
+        <f t="shared" si="1"/>
+        <v>8.5336459973587298E-2</v>
+      </c>
+      <c r="H13" s="155">
+        <v>500035962</v>
+      </c>
+      <c r="I13" s="157">
+        <f t="shared" si="2"/>
+        <v>0.1093519651658541</v>
+      </c>
+      <c r="J13" s="157">
+        <f t="shared" si="0"/>
+        <v>0.79451530173529694</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2015</v>
+      </c>
+      <c r="D14" s="154">
+        <v>2016</v>
+      </c>
+      <c r="F14" s="155">
+        <f>623414600-563500 + 4237083</f>
+        <v>627088183</v>
+      </c>
+      <c r="G14" s="157">
+        <f t="shared" si="1"/>
+        <v>-3.6093505393035574E-3</v>
+      </c>
+      <c r="H14" s="155">
+        <v>554863405</v>
+      </c>
+      <c r="I14" s="157">
+        <f t="shared" si="2"/>
+        <v>0.10964699974919001</v>
+      </c>
+      <c r="J14" s="157">
+        <f t="shared" si="0"/>
+        <v>0.88482516501191988</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="155"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>